<commit_message>
se agrega el bat
</commit_message>
<xml_diff>
--- a/credenciales.xlsx
+++ b/credenciales.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUAWEI\Desktop\Credencializacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDB791D-D05C-41E4-806B-917C53DD886D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD209B38-A158-473B-B89C-79A3C557FAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{DAEBF4EF-2D0A-4BA3-9620-C7324F5F902D}"/>
   </bookViews>
@@ -34,40 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
-  <si>
-    <t>text1</t>
-  </si>
-  <si>
-    <t>text2</t>
-  </si>
-  <si>
-    <t>text3</t>
-  </si>
-  <si>
-    <t>text4</t>
-  </si>
-  <si>
-    <t>text5</t>
-  </si>
-  <si>
-    <t>text6</t>
-  </si>
-  <si>
-    <t>text7</t>
-  </si>
-  <si>
-    <t>text8</t>
-  </si>
-  <si>
-    <t>text9</t>
-  </si>
-  <si>
-    <t>text10</t>
-  </si>
-  <si>
-    <t>text11</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Gerente de Operaciones</t>
   </si>
@@ -148,6 +115,42 @@
   </si>
   <si>
     <t>Santiago Montejo</t>
+  </si>
+  <si>
+    <t>puesto</t>
+  </si>
+  <si>
+    <t>curp</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>alergia</t>
+  </si>
+  <si>
+    <t>fecha_expedicion</t>
+  </si>
+  <si>
+    <t>tipo_sangre</t>
+  </si>
+  <si>
+    <t>fecha_vigencia</t>
+  </si>
+  <si>
+    <t>familiar</t>
+  </si>
+  <si>
+    <t>parentesco</t>
+  </si>
+  <si>
+    <t>telefono_parentesco</t>
+  </si>
+  <si>
+    <t>nombre_elemento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url_imagen </t>
   </si>
 </sst>
 </file>
@@ -536,75 +539,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2731DF9A-63CC-4C0B-B2FC-9FF25C4759CB}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="2">
         <v>98765432100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3">
         <v>45861</v>
@@ -613,33 +619,33 @@
         <v>47322</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C3" s="2">
         <v>12345678900</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3">
         <v>45861</v>
@@ -648,33 +654,33 @@
         <v>47322</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2">
         <v>45678912300</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3">
         <v>45861</v>
@@ -683,33 +689,33 @@
         <v>47322</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
         <v>98765432103</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F5" s="3">
         <v>45861</v>
@@ -718,33 +724,33 @@
         <v>47322</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>98765432103</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3">
         <v>45861</v>
@@ -753,33 +759,33 @@
         <v>47322</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
         <v>98765432103</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F7" s="3">
         <v>45861</v>
@@ -788,16 +794,16 @@
         <v>47322</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>